<commit_message>
update to include isoforms in normalisation table issue #9
</commit_message>
<xml_diff>
--- a/docs/normalisation_thoughts/normalisation_database.xlsx
+++ b/docs/normalisation_thoughts/normalisation_database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livelancsac-my.sharepoint.com/personal/monserrj_lancaster_ac_uk/Documents/Project - JMR/2. Experiments/6. Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monserrj\1.BMC\BMC-database-1\docs\normalisation_thoughts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A124DD-E21B-460E-9759-F31246F7922D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9DA3A7-E958-4996-BACB-F963694C11A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>tc={8225B6DE-5319-428D-90CE-8EDEFF5C5865}</author>
   </authors>
   <commentList>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
+    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -38,7 +38,7 @@
     do I want the origin organism for the modfied versions, I think it is useful information but may cause confusion</t>
       </text>
     </comment>
-    <comment ref="L8" authorId="1" shapeId="0" xr:uid="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
+    <comment ref="N8" authorId="1" shapeId="0" xr:uid="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +47,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="S18" authorId="2" shapeId="0" xr:uid="{9DB239A6-8497-4387-833D-57D2AED81F35}">
+    <comment ref="U18" authorId="2" shapeId="0" xr:uid="{9DB239A6-8497-4387-833D-57D2AED81F35}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="N33" authorId="3" shapeId="0" xr:uid="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
+    <comment ref="P33" authorId="3" shapeId="0" xr:uid="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     KEGG: related genes, papers, function</t>
       </text>
     </comment>
-    <comment ref="X44" authorId="4" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
+    <comment ref="Z44" authorId="4" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="166">
   <si>
     <t>prot_seq</t>
   </si>
@@ -576,13 +576,22 @@
   </si>
   <si>
     <t>Leave it aside for now until the database is in a better shape</t>
+  </si>
+  <si>
+    <t>is_canonical</t>
+  </si>
+  <si>
+    <t>Isoform</t>
+  </si>
+  <si>
+    <t>canonical_prot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -757,12 +766,6 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1151,18 +1154,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" xfId="6" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="6" applyFont="1"/>
@@ -1171,12 +1170,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1186,15 +1180,15 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="28" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="27" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1576,30 +1570,30 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="O6" dT="2025-05-13T14:16:04.33" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
+  <threadedComment ref="Q6" dT="2025-05-13T14:16:04.33" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
     <text>do I want the origin organism for the modfied versions, I think it is useful information but may cause confusion</text>
   </threadedComment>
-  <threadedComment ref="L8" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
+  <threadedComment ref="N8" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
     <text xml:space="preserve">Would it be null as it comes from a modified version or would I want it still on comments?
 </text>
   </threadedComment>
-  <threadedComment ref="S18" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{9DB239A6-8497-4387-833D-57D2AED81F35}">
+  <threadedComment ref="U18" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{9DB239A6-8497-4387-833D-57D2AED81F35}">
     <text xml:space="preserve">Would it be null as it comes from a modified version or would I want it still on comments?
 </text>
   </threadedComment>
-  <threadedComment ref="N33" dT="2025-05-13T14:24:47.02" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
+  <threadedComment ref="P33" dT="2025-05-13T14:24:47.02" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
     <text>Uniprot: Gives you references to other ext database, with info about org, strct,seq,gene… if available</text>
   </threadedComment>
-  <threadedComment ref="N33" dT="2025-05-13T14:25:55.58" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{898593B5-CDAB-42AD-B278-9494D9C6EB25}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
+  <threadedComment ref="P33" dT="2025-05-13T14:25:55.58" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{898593B5-CDAB-42AD-B278-9494D9C6EB25}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
     <text>NCBI: locus, organism, paper of discovery, sequence, aa sequence</text>
   </threadedComment>
-  <threadedComment ref="N33" dT="2025-05-13T14:28:39.79" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{A3FBD037-F5C0-46B7-85F2-EE850E637A4F}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
+  <threadedComment ref="P33" dT="2025-05-13T14:28:39.79" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{A3FBD037-F5C0-46B7-85F2-EE850E637A4F}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
     <text>GO: uniprot ref, function , taxon, synonyms of function type, papers with reference to function and protein</text>
   </threadedComment>
-  <threadedComment ref="N33" dT="2025-05-13T14:30:14.15" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{62240600-B1E7-44E6-B96A-5BEA743DB408}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
+  <threadedComment ref="P33" dT="2025-05-13T14:30:14.15" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{62240600-B1E7-44E6-B96A-5BEA743DB408}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
     <text>KEGG: related genes, papers, function</text>
   </threadedComment>
-  <threadedComment ref="X44" dT="2025-05-13T14:08:36.10" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
+  <threadedComment ref="Z44" dT="2025-05-13T14:08:36.10" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
     <text xml:space="preserve">Unsure as you can make many modifications to the same DNA sequence if I can add them all to the same protein (maybe like the pdb?)
 </text>
   </threadedComment>
@@ -1608,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783CC8DE-7F76-644C-B681-A92CC700BEB1}">
-  <dimension ref="A1:Z83"/>
+  <dimension ref="A1:AB83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1619,12 +1613,12 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="13" max="13" width="7.4140625" customWidth="1"/>
+    <col min="5" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="15" max="15" width="7.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,68 +1634,74 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="W1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1717,24 +1717,24 @@
       <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1744,41 +1744,47 @@
       <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="1">
         <v>502025</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1794,24 +1800,24 @@
       <c r="E3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="I3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L3" s="1" t="s">
         <v>53</v>
       </c>
@@ -1821,41 +1827,47 @@
       <c r="N3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="1">
         <v>99287</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="S3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3" s="8">
         <v>3</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1871,24 +1883,24 @@
       <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1898,41 +1910,47 @@
       <c r="N4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="1">
         <v>546</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="12">
+      <c r="S4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="8">
         <v>6</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1948,24 +1966,24 @@
       <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="I5" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L5" s="1" t="s">
         <v>53</v>
       </c>
@@ -1975,41 +1993,47 @@
       <c r="N5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" s="1">
         <v>99287</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="S5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" s="8">
         <v>3</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2025,24 +2049,24 @@
       <c r="E6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="I6" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L6" s="1" t="s">
         <v>53</v>
       </c>
@@ -2052,251 +2076,269 @@
       <c r="N6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="1">
         <v>546</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="S6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W6" s="8">
         <v>6</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="Y6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="I7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="J7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="K7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J7" s="13">
+      <c r="L7" s="1">
         <v>4</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="M7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="N7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="O7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="P7" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <v>546</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="S7" s="1" t="s">
         <v>53</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W7" s="8">
         <v>6</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="Y7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="I8" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="J8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="K8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="13">
+      <c r="L8" s="1">
         <v>5</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="M8" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="10" t="s">
+      <c r="N8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="1">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1">
         <v>546</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="S8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="12">
+      <c r="U8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W8" s="8">
         <v>6</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="Y8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G11" s="2" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="M12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="1"/>
+      <c r="P12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -2306,48 +2348,51 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="M13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="N13" s="1"/>
+      <c r="P13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U13" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="T13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -2357,48 +2402,51 @@
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="1">
+      <c r="D14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
         <v>2</v>
       </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="M14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="N14" s="1">
+      <c r="N14" s="1"/>
+      <c r="P14" s="1">
         <v>2</v>
       </c>
-      <c r="O14" s="1">
+      <c r="Q14" s="1">
         <v>2</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="T14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U14" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="T14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -2408,48 +2456,51 @@
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="1">
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
         <v>3</v>
       </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="M15" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="N15" s="1">
+      <c r="N15" s="1"/>
+      <c r="P15" s="1">
         <v>3</v>
       </c>
-      <c r="O15" s="1">
+      <c r="Q15" s="1">
         <v>3</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="T15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U15" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="T15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -2459,163 +2510,169 @@
       <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="1">
+      <c r="D16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
         <v>4</v>
       </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="M16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="N16" s="1">
+      <c r="N16" s="1"/>
+      <c r="P16" s="1">
         <v>4</v>
       </c>
-      <c r="O16" s="1">
+      <c r="Q16" s="1">
         <v>4</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R16" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S16" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="T16" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U16" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A17" s="11">
+      <c r="T16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A17" s="7">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="1">
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
         <v>5</v>
       </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="M17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="N17" s="1">
+      <c r="N17" s="1"/>
+      <c r="P17" s="1">
         <v>5</v>
       </c>
-      <c r="O17" s="1">
+      <c r="Q17" s="1">
         <v>4</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="R17" s="27" t="s">
+      <c r="T17" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="S17" s="27" t="s">
+      <c r="U17" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="T17" s="28" t="s">
+      <c r="V17" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="U17" s="28" t="s">
+      <c r="W17" s="21" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="G18" s="1">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="I18" s="1">
         <v>6</v>
       </c>
-      <c r="H18" s="1">
+      <c r="J18" s="1">
         <v>2</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="M18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="N18" s="1">
+      <c r="N18" s="1"/>
+      <c r="P18" s="1">
         <v>6</v>
       </c>
-      <c r="O18" s="1">
+      <c r="Q18" s="1">
         <v>4</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="R18" s="27" t="s">
+      <c r="T18" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="S18" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="T18" s="28" t="s">
+      <c r="U18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="V18" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="U18" s="28"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="W18" s="21"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="1">
+      <c r="I19" s="1">
         <v>7</v>
       </c>
-      <c r="H19" s="1">
+      <c r="J19" s="1">
         <v>2</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="M19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2628,27 +2685,29 @@
       <c r="E20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="1">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20" s="1">
         <v>8</v>
       </c>
-      <c r="H20" s="1">
+      <c r="J20" s="1">
         <v>2</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="M20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="N20" s="2" t="s">
+      <c r="N20" s="1"/>
+      <c r="P20" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -2661,42 +2720,44 @@
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="1">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="I21" s="1">
         <v>9</v>
       </c>
-      <c r="H21" s="1">
+      <c r="J21" s="1">
         <v>2</v>
       </c>
-      <c r="I21" s="1">
+      <c r="K21" s="1">
         <v>31469</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="M21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="N21" s="1" t="s">
+      <c r="N21" s="1"/>
+      <c r="P21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="R21" s="13" t="s">
+      <c r="T21" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -2709,42 +2770,44 @@
       <c r="E22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="1">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="I22" s="1">
         <v>10</v>
       </c>
-      <c r="H22" s="1">
+      <c r="J22" s="1">
         <v>3</v>
       </c>
-      <c r="I22" s="1">
+      <c r="K22" s="1">
         <v>78900</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="M22" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="N22" s="1">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1</v>
-      </c>
+      <c r="N22" s="1"/>
       <c r="P22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
         <v>502025</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="T22" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -2757,42 +2820,44 @@
       <c r="E23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="1">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="I23" s="1">
         <v>11</v>
       </c>
-      <c r="H23" s="1">
+      <c r="J23" s="1">
         <v>3</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="M23" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="N23" s="1">
+      <c r="N23" s="1"/>
+      <c r="P23" s="1">
         <v>2</v>
       </c>
-      <c r="O23" s="1">
+      <c r="Q23" s="1">
         <v>2</v>
       </c>
-      <c r="P23" s="1">
+      <c r="R23" s="1">
         <v>99287</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="T23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="X23" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -2805,39 +2870,41 @@
       <c r="E24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G24" s="1">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="I24" s="1">
         <v>12</v>
       </c>
-      <c r="H24" s="1">
+      <c r="J24" s="1">
         <v>3</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="K24" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="L24" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="M24" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="N24" s="1">
+      <c r="N24" s="1"/>
+      <c r="P24" s="1">
         <v>3</v>
       </c>
-      <c r="O24" s="1">
+      <c r="Q24" s="1">
         <v>3</v>
       </c>
-      <c r="P24" s="1">
+      <c r="R24" s="1">
         <v>546</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="T24" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -2850,165 +2917,184 @@
       <c r="E25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="1">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="I25" s="1">
         <v>13</v>
       </c>
-      <c r="H25" s="1">
+      <c r="J25" s="1">
         <v>3</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="K25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="L25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="M25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="N25" s="1">
+      <c r="N25" s="1"/>
+      <c r="P25" s="1">
         <v>4</v>
       </c>
-      <c r="O25" s="1">
+      <c r="Q25" s="1">
         <v>3</v>
       </c>
-      <c r="P25" s="1">
+      <c r="R25" s="1">
         <v>546</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R25" s="13" t="s">
+      <c r="T25" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V25" s="1" t="s">
+      <c r="X25" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="G26" s="1">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="I26" s="1">
         <v>14</v>
       </c>
-      <c r="H26" s="1">
+      <c r="J26" s="1">
         <v>4</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="13" t="s">
+      <c r="M26" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N26" s="1">
+      <c r="P26" s="1">
         <v>5</v>
       </c>
-      <c r="O26" s="1">
+      <c r="Q26" s="1">
         <v>3</v>
       </c>
-      <c r="P26" s="1">
+      <c r="R26" s="1">
         <v>546</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R26" s="13" t="s">
+      <c r="T26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V26" s="1" t="s">
+      <c r="X26" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="G27" s="1">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="I27" s="1">
         <v>15</v>
       </c>
-      <c r="H27" s="1">
+      <c r="J27" s="1">
         <v>4</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="M27" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="1">
+      <c r="P27" s="1">
         <v>6</v>
       </c>
-      <c r="O27" s="1">
+      <c r="Q27" s="1">
         <v>3</v>
       </c>
-      <c r="P27" s="1">
+      <c r="R27" s="1">
         <v>546</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="T27" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="G28" s="1">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="D28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I28" s="1">
         <v>16</v>
       </c>
-      <c r="H28" s="1">
+      <c r="J28" s="1">
         <v>4</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="K28" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="L28" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="M28" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="G29" s="1">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="D29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I29" s="1">
         <v>17</v>
       </c>
-      <c r="H29" s="1">
+      <c r="J29" s="1">
         <v>4</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="K29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="L29" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="M29" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N33" s="15" t="s">
+      <c r="P33" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="T33" s="2" t="s">
+      <c r="V33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Y33" s="2" t="s">
+      <c r="AA33" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -3018,50 +3104,53 @@
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="D34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T34" s="1" t="s">
+      <c r="V34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="U34" s="1" t="s">
+      <c r="W34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="V34" s="1" t="s">
+      <c r="X34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="X34" s="1" t="s">
+      <c r="Z34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Y34" s="1" t="s">
+      <c r="AA34" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Z34" s="1" t="s">
+      <c r="AB34" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -3071,56 +3160,59 @@
       <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="D35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K35" s="1">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1">
+      <c r="M35" s="1">
         <v>1</v>
       </c>
       <c r="N35" s="1">
         <v>1</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="S35" s="1">
-        <v>1</v>
-      </c>
-      <c r="T35" s="1">
-        <v>1</v>
-      </c>
-      <c r="U35" s="1" t="s">
+      <c r="U35" s="1">
+        <v>1</v>
+      </c>
+      <c r="V35" s="1">
+        <v>1</v>
+      </c>
+      <c r="W35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V35" s="1" t="s">
+      <c r="X35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X35" s="1">
+      <c r="Z35" s="1">
         <v>5</v>
       </c>
-      <c r="Y35" s="1" t="s">
+      <c r="AA35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="Z35" s="1" t="s">
+      <c r="AB35" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -3130,56 +3222,59 @@
       <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="1">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1" t="s">
+      <c r="D36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I36" s="1">
-        <v>1</v>
-      </c>
       <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="1">
         <v>2</v>
       </c>
-      <c r="L36" s="1">
-        <v>1</v>
-      </c>
       <c r="N36" s="1">
+        <v>1</v>
+      </c>
+      <c r="P36" s="1">
         <v>2</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="S36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="S36" s="1">
+      <c r="U36" s="1">
         <v>2</v>
       </c>
-      <c r="T36" s="1">
+      <c r="V36" s="1">
         <v>2</v>
       </c>
-      <c r="U36" s="1" t="s">
+      <c r="W36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="V36" s="1" t="s">
+      <c r="X36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X36" s="1">
+      <c r="Z36" s="1">
         <v>6</v>
       </c>
-      <c r="Y36" s="1" t="s">
+      <c r="AA36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Z36" s="1" t="s">
+      <c r="AB36" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -3189,229 +3284,235 @@
       <c r="C37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="1">
-        <v>2</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>22</v>
+      <c r="D37" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="I37" s="1">
         <v>2</v>
       </c>
+      <c r="J37" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K37" s="1">
+        <v>2</v>
+      </c>
+      <c r="M37" s="1">
         <v>3</v>
       </c>
-      <c r="L37" s="1">
-        <v>1</v>
-      </c>
       <c r="N37" s="1">
+        <v>1</v>
+      </c>
+      <c r="P37" s="1">
         <v>3</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="S37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S37" s="1">
+      <c r="U37" s="1">
         <v>3</v>
       </c>
-      <c r="T37" s="1">
+      <c r="V37" s="1">
         <v>3</v>
       </c>
-      <c r="U37" s="1" t="s">
+      <c r="W37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V37" s="1" t="s">
+      <c r="X37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X37" s="1">
+      <c r="Z37" s="1">
         <v>5</v>
       </c>
-      <c r="Y37" s="1" t="s">
+      <c r="AA37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="Z37" s="1" t="s">
+      <c r="AB37" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A38" s="11">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A38" s="7">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="1">
-        <v>3</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>27</v>
+      <c r="D38" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I38" s="1">
         <v>3</v>
       </c>
+      <c r="J38" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K38" s="1">
+        <v>3</v>
+      </c>
+      <c r="M38" s="1">
         <v>4</v>
       </c>
-      <c r="L38" s="1">
-        <v>1</v>
-      </c>
       <c r="N38" s="1">
+        <v>1</v>
+      </c>
+      <c r="P38" s="1">
         <v>4</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="S38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S38" s="1">
+      <c r="U38" s="1">
         <v>4</v>
       </c>
-      <c r="T38" s="1">
+      <c r="V38" s="1">
         <v>4</v>
       </c>
-      <c r="U38" s="1" t="s">
+      <c r="W38" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="V38" s="1" t="s">
+      <c r="X38" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="G39" s="1">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="I39" s="1">
         <v>4</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="1">
+      <c r="K39" s="1">
         <v>3</v>
       </c>
-      <c r="K39" s="1">
+      <c r="M39" s="1">
         <v>5</v>
       </c>
-      <c r="L39" s="1">
-        <v>1</v>
-      </c>
       <c r="N39" s="1">
+        <v>1</v>
+      </c>
+      <c r="P39" s="1">
         <v>5</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="S39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S39" s="1">
+      <c r="U39" s="1">
         <v>5</v>
       </c>
-      <c r="T39" s="1">
+      <c r="V39" s="1">
         <v>4</v>
       </c>
-      <c r="U39" s="1" t="s">
+      <c r="W39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="V39" s="1" t="s">
+      <c r="X39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="X39" s="23" t="s">
+      <c r="Z39" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="Y39" s="23" t="s">
+      <c r="AA39" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="G40" s="1">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="I40" s="1">
         <v>5</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I40" s="1">
+      <c r="K40" s="1">
         <v>4</v>
       </c>
-      <c r="K40" s="1">
+      <c r="M40" s="1">
         <v>6</v>
       </c>
-      <c r="L40" s="1">
+      <c r="N40" s="1">
         <v>2</v>
       </c>
-      <c r="N40" s="1">
+      <c r="P40" s="1">
         <v>6</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="S40" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="S40" s="1">
+      <c r="U40" s="1">
         <v>6</v>
       </c>
-      <c r="T40" s="1">
+      <c r="V40" s="1">
         <v>4</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="W40" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="V40" s="1" t="s">
+      <c r="X40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="X40" s="24" t="s">
+      <c r="Z40" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="Y40" s="25" t="s">
+      <c r="AA40" s="18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="1">
+      <c r="I41" s="1">
         <v>6</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="1">
-        <v>1</v>
-      </c>
       <c r="K41" s="1">
+        <v>1</v>
+      </c>
+      <c r="M41" s="1">
         <v>7</v>
       </c>
-      <c r="L41" s="1">
+      <c r="N41" s="1">
         <v>2</v>
       </c>
-      <c r="X41" s="24" t="s">
+      <c r="Z41" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="Y41" s="25" t="s">
+      <c r="AA41" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
@@ -3424,36 +3525,38 @@
       <c r="E42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G42" s="1">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="I42" s="1">
         <v>7</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="1">
+      <c r="K42" s="1">
         <v>2</v>
       </c>
-      <c r="K42" s="1">
+      <c r="M42" s="1">
         <v>8</v>
       </c>
-      <c r="L42" s="1">
+      <c r="N42" s="1">
         <v>2</v>
       </c>
-      <c r="N42" s="7" t="s">
+      <c r="P42" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="O42" s="7"/>
-      <c r="T42" s="2" t="s">
+      <c r="Q42" s="6"/>
+      <c r="V42" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="X42" s="24" t="s">
+      <c r="Z42" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="Y42" s="25" t="s">
+      <c r="AA42" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -3466,41 +3569,43 @@
       <c r="E43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="1">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="I43" s="1">
         <v>8</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I43" s="1">
+      <c r="K43" s="1">
         <v>5</v>
       </c>
-      <c r="K43" s="1">
+      <c r="M43" s="1">
         <v>9</v>
       </c>
-      <c r="L43" s="1">
+      <c r="N43" s="1">
         <v>2</v>
       </c>
-      <c r="N43" s="7" t="s">
+      <c r="P43" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="O43" s="7" t="s">
+      <c r="Q43" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="V43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="U43" s="1" t="s">
+      <c r="W43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V43" s="1" t="s">
+      <c r="X43" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -3513,47 +3618,49 @@
       <c r="E44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G44" s="1">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="I44" s="1">
         <v>9</v>
       </c>
-      <c r="H44" s="1">
+      <c r="J44" s="1">
         <v>31469</v>
       </c>
-      <c r="I44" s="1">
+      <c r="K44" s="1">
         <v>4</v>
       </c>
-      <c r="K44" s="1">
+      <c r="M44" s="1">
         <v>10</v>
       </c>
-      <c r="L44" s="1">
+      <c r="N44" s="1">
         <v>3</v>
       </c>
-      <c r="N44" s="7" t="s">
+      <c r="P44" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="O44" s="7" t="s">
+      <c r="Q44" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="S44" s="1">
-        <v>1</v>
-      </c>
-      <c r="T44" s="1">
-        <v>1</v>
-      </c>
       <c r="U44" s="1">
+        <v>1</v>
+      </c>
+      <c r="V44" s="1">
+        <v>1</v>
+      </c>
+      <c r="W44" s="1">
         <v>502025</v>
       </c>
-      <c r="V44" s="1">
+      <c r="X44" s="1">
         <v>6</v>
       </c>
-      <c r="X44" s="26" t="s">
+      <c r="Z44" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="Y44" s="23" t="s">
+      <c r="AA44" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -3566,47 +3673,49 @@
       <c r="E45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G45" s="1">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="I45" s="1">
         <v>10</v>
       </c>
-      <c r="H45" s="1">
+      <c r="J45" s="1">
         <v>78900</v>
       </c>
-      <c r="I45" s="1">
-        <v>1</v>
-      </c>
       <c r="K45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
         <v>11</v>
       </c>
-      <c r="L45" s="1">
+      <c r="N45" s="1">
         <v>3</v>
       </c>
-      <c r="N45" s="7" t="s">
+      <c r="P45" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="O45" s="7" t="s">
+      <c r="Q45" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="S45" s="1">
+      <c r="U45" s="1">
         <v>2</v>
       </c>
-      <c r="T45" s="1">
+      <c r="V45" s="1">
         <v>2</v>
       </c>
-      <c r="U45" s="1">
+      <c r="W45" s="1">
         <v>99287</v>
       </c>
-      <c r="V45" s="1">
+      <c r="X45" s="1">
         <v>6</v>
       </c>
-      <c r="X45" s="24" t="s">
+      <c r="Z45" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Y45" s="25" t="s">
+      <c r="AA45" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -3619,47 +3728,49 @@
       <c r="E46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="1">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="I46" s="1">
         <v>11</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I46" s="1">
+      <c r="K46" s="1">
         <v>2</v>
       </c>
-      <c r="K46" s="1">
+      <c r="M46" s="1">
         <v>12</v>
       </c>
-      <c r="L46" s="1">
+      <c r="N46" s="1">
         <v>3</v>
       </c>
-      <c r="N46" s="7" t="s">
+      <c r="P46" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="O46" s="7" t="s">
+      <c r="Q46" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="S46" s="1">
+      <c r="U46" s="1">
         <v>3</v>
       </c>
-      <c r="T46" s="1">
+      <c r="V46" s="1">
         <v>3</v>
       </c>
-      <c r="U46" s="1">
+      <c r="W46" s="1">
         <v>546</v>
       </c>
-      <c r="V46" s="1">
+      <c r="X46" s="1">
         <v>6</v>
       </c>
-      <c r="X46" s="24" t="s">
+      <c r="Z46" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="Y46" s="25" t="s">
+      <c r="AA46" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>4</v>
       </c>
@@ -3672,373 +3783,356 @@
       <c r="E47" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G47" s="1">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="I47" s="1">
         <v>12</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I47" s="1">
+      <c r="K47" s="1">
         <v>5</v>
       </c>
-      <c r="K47" s="1">
+      <c r="M47" s="1">
         <v>13</v>
       </c>
-      <c r="L47" s="1">
+      <c r="N47" s="1">
         <v>3</v>
       </c>
-      <c r="S47" s="1">
+      <c r="U47" s="1">
         <v>4</v>
       </c>
-      <c r="T47" s="1">
+      <c r="V47" s="1">
         <v>4</v>
       </c>
-      <c r="U47" s="1">
+      <c r="W47" s="1">
         <v>546</v>
       </c>
-      <c r="V47" s="1">
+      <c r="X47" s="1">
         <v>6</v>
       </c>
-      <c r="X47" s="24" t="s">
+      <c r="Z47" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="Y47" s="25" t="s">
+      <c r="AA47" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="G48" s="1">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="I48" s="1">
         <v>13</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I48" s="1">
+      <c r="K48" s="1">
         <v>4</v>
       </c>
-      <c r="K48" s="1">
+      <c r="M48" s="1">
         <v>14</v>
       </c>
-      <c r="L48" s="1">
+      <c r="N48" s="1">
         <v>4</v>
       </c>
-      <c r="S48" s="1">
+      <c r="U48" s="1">
         <v>5</v>
       </c>
-      <c r="T48" s="1">
+      <c r="V48" s="1">
         <v>5</v>
       </c>
-      <c r="U48" s="1">
+      <c r="W48" s="1">
         <v>546</v>
       </c>
-      <c r="V48" s="1">
+      <c r="X48" s="1">
         <v>6</v>
       </c>
-      <c r="X48" s="24" t="s">
+      <c r="Z48" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="Y48" s="25" t="s">
+      <c r="AA48" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G49" s="1">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="D49" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I49" s="1">
         <v>14</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I49" s="1">
-        <v>1</v>
-      </c>
       <c r="K49" s="1">
+        <v>1</v>
+      </c>
+      <c r="M49" s="1">
         <v>15</v>
       </c>
-      <c r="L49" s="1">
+      <c r="N49" s="1">
         <v>4</v>
       </c>
-      <c r="S49" s="1">
+      <c r="U49" s="1">
         <v>6</v>
-      </c>
-      <c r="T49" s="1">
-        <v>6</v>
-      </c>
-      <c r="U49" s="1">
-        <v>546</v>
       </c>
       <c r="V49" s="1">
         <v>6</v>
       </c>
-      <c r="X49" s="24" t="s">
+      <c r="W49" s="1">
+        <v>546</v>
+      </c>
+      <c r="X49" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z49" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="Y49" s="25" t="s">
+      <c r="AA49" s="18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G50" s="1">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="D50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I50" s="1">
         <v>15</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I50" s="1">
+      <c r="K50" s="1">
         <v>2</v>
       </c>
-      <c r="K50" s="1">
+      <c r="M50" s="1">
         <v>12</v>
       </c>
-      <c r="L50" s="1">
+      <c r="N50" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="K51" s="1">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="D51" s="1">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4</v>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="M51" s="1">
         <v>13</v>
       </c>
-      <c r="L51" s="1">
+      <c r="N51" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A53" s="5"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="18"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G57" s="20"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G58" s="20"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G59" s="20"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G60" s="20"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G61" s="20"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G62" s="20"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G63" s="20"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="G64" s="20"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G65" s="20"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G66" s="20"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="20"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G67" s="20"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="20"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="19"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="20"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="19"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="20"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A70" s="19"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A71" s="18"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="20"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="19"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="20"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="20"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="19"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="20"/>
-      <c r="J73" s="20"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="19"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
-      <c r="J75" s="19"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="19"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="19"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="20"/>
-      <c r="H77" s="20"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="19"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
-    </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="20"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
-      <c r="J81" s="19"/>
-    </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-      <c r="J82" s="19"/>
-    </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.4">
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
-      <c r="J83" s="19"/>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="I64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A71" s="14"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="12"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+    </row>
+    <row r="81" spans="5:9" x14ac:dyDescent="0.4">
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+    </row>
+    <row r="82" spans="5:9" x14ac:dyDescent="0.4">
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+    </row>
+    <row r="83" spans="5:9" x14ac:dyDescent="0.4">
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="25" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -4056,180 +4150,180 @@
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="30">
-        <v>1</v>
-      </c>
-      <c r="B5" s="32">
+      <c r="A5" s="23">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25">
         <v>45783</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="24" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="30">
-        <v>1</v>
-      </c>
-      <c r="B10" s="30">
-        <v>1</v>
-      </c>
-      <c r="C10" s="30" t="s">
+      <c r="A10" s="23">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23">
+        <v>1</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="30">
-        <v>1</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="30">
+      <c r="A11" s="23">
         <v>2</v>
       </c>
-      <c r="B11" s="30">
-        <v>1</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="23">
+        <v>1</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="23">
         <v>3.5</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" s="30">
+      <c r="A12" s="23">
         <v>3</v>
       </c>
-      <c r="B12" s="30">
-        <v>1</v>
-      </c>
-      <c r="C12" s="30" t="s">
+      <c r="B12" s="23">
+        <v>1</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="30"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" s="30">
+      <c r="A13" s="23">
         <v>3</v>
       </c>
-      <c r="B13" s="30">
-        <v>1</v>
-      </c>
-      <c r="C13" s="30" t="s">
+      <c r="B13" s="23">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="30"/>
+      <c r="F13" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update of excel with comments after meeting with Leighton
</commit_message>
<xml_diff>
--- a/docs/normalisation_thoughts/normalisation_database.xlsx
+++ b/docs/normalisation_thoughts/normalisation_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monserrj\1.BMC\BMC-database-1\docs\normalisation_thoughts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C754192-C794-4AE8-B284-E409BBD27E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347A3A6-172E-4FA9-ACCC-64077C8034AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="prot_data_minimal_correct" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <author>tc={91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}</author>
     <author>tc={9DB239A6-8497-4387-833D-57D2AED81F35}</author>
     <author>tc={189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}</author>
+    <author>tc={DF0AE6F2-F317-4F6F-AF56-764C13C56519}</author>
     <author>tc={03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}</author>
     <author>tc={60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}</author>
     <author>tc={8225B6DE-5319-428D-90CE-8EDEFF5C5865}</author>
@@ -38,16 +39,19 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    do I want the origin organism for the modfied versions, I think it is useful information but may cause confusion</t>
+    do I want the origin organism for the modfied versions, I think it is useful information but may cause confusion
+Reply:
+    If unchange sequence reasonable, when modifie no tax</t>
       </text>
     </comment>
     <comment ref="Y8" authorId="1" shapeId="0" xr:uid="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Would it be null as it comes from a modified version or would I want it still on comments?
-</t>
+Reply:
+    fine</t>
       </text>
     </comment>
     <comment ref="S19" authorId="2" shapeId="0" xr:uid="{9DB239A6-8497-4387-833D-57D2AED81F35}">
@@ -73,7 +77,15 @@
     KEGG: related genes, papers, function</t>
       </text>
     </comment>
-    <comment ref="V39" authorId="4" shapeId="0" xr:uid="{03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}">
+    <comment ref="W38" authorId="4" shapeId="0" xr:uid="{DF0AE6F2-F317-4F6F-AF56-764C13C56519}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dentifer for engineering change sequence that inmediately preceds it</t>
+      </text>
+    </comment>
+    <comment ref="V39" authorId="5" shapeId="0" xr:uid="{03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +93,7 @@
     Add condition that if origin true origin_cds null?</t>
       </text>
     </comment>
-    <comment ref="P60" authorId="5" shapeId="0" xr:uid="{60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}">
+    <comment ref="P60" authorId="6" shapeId="0" xr:uid="{60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +101,7 @@
     Check this change</t>
       </text>
     </comment>
-    <comment ref="N65" authorId="6" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
+    <comment ref="N65" authorId="7" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,6 +117,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={AEC729A6-7C26-49DC-9714-BAA59955DFAE}</author>
     <author>tc={0F9AD2A1-2F87-43BD-9092-A77977442708}</author>
     <author>tc={7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}</author>
     <author>tc={EF411826-7395-4077-8E4B-D55F86DAD678}</author>
@@ -113,7 +126,45 @@
     <author>tc={2B9A8B6C-00AD-4E85-91E5-666B4DFA8621}</author>
   </authors>
   <commentList>
-    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{AEC729A6-7C26-49DC-9714-BAA59955DFAE}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Describe the complex in what type of interaction (beisbl ball example), Represent how individal members interact with each other. 
+Reply:
+    Have 2 queries when searching for information and remove repetition, also make interaction depending on complex 
+Reply:
+     </t>
+      </text>
+    </comment>
+    <comment ref="AB33" authorId="1" shapeId="0" xr:uid="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Unsure about this being clear enough, comment on native example
+Reply:
+    Pdu, HO compare and decide which one that gives me unique information.
+Reply:
+    Definition of complex that reflects the differences so I have the categories and therefore I can put differences between pdue and eut
+Reply:
+    Leave it aside for now and we can apply it later on</t>
+      </text>
+    </comment>
+    <comment ref="G54" authorId="2" shapeId="0" xr:uid="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I know what I want to do, but not sure how to sestablish nomenclature. As this is a if prot_id_1 interacts with prot_id_2 then I don’t need to add that prot_id_2 interacts with prot_id_1
+Reply:
+    Also this table is like apart from the others in the same that I think I don’t want it related to the complex as the porteins interacts with those, so I know that, that prot 1 interacts with 2 and 3, and I know what the complex is made of so if it has 2 but not 3 is quite obvious what is interacting. Does that make sense?
+Reply:
+    Interactions 2 spearate categories? EP core and shell structure for assembly?</t>
+      </text>
+    </comment>
+    <comment ref="L54" authorId="3" shapeId="0" xr:uid="{EF411826-7395-4077-8E4B-D55F86DAD678}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -122,26 +173,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="F54" authorId="1" shapeId="0" xr:uid="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I know what I want to do, but not sure how to sestablish nomenclature. As this is a if prot_id_1 interacts with prot_id_2 then I don’t need to add that prot_id_2 interacts with prot_id_1
-Reply:
-    Also this table is like apart from the others in the same that I think I don’t want it related to the complex as the porteins interacts with those, so I know that, that prot 1 interacts with 2 and 3, and I know what the complex is made of so if it has 2 but not 3 is quite obvious what is interacting. Does that make sense?</t>
-      </text>
-    </comment>
-    <comment ref="L54" authorId="2" shapeId="0" xr:uid="{EF411826-7395-4077-8E4B-D55F86DAD678}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Unsure about this being clear enough, comment on native example
-</t>
-      </text>
-    </comment>
-    <comment ref="O61" authorId="3" shapeId="0" xr:uid="{7C330DC9-65D1-4AD0-8266-2618258CAE0B}">
+    <comment ref="O61" authorId="4" shapeId="0" xr:uid="{7C330DC9-65D1-4AD0-8266-2618258CAE0B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -151,15 +183,17 @@
     Work in progress</t>
       </text>
     </comment>
-    <comment ref="J69" authorId="4" shapeId="0" xr:uid="{237F9E53-A724-461A-9D97-96190E1F43BA}">
+    <comment ref="J69" authorId="5" shapeId="0" xr:uid="{237F9E53-A724-461A-9D97-96190E1F43BA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    This is not needed for database is so I can make sense in my head with the names I give to things, or would it be helpful? Names may be repeated by type but I do use them for experimental purposes when naming constructs</t>
+    This is not needed for database is so I can make sense in my head with the names I give to things, or would it be helpful? Names may be repeated by type but I do use them for experimental purposes when naming constructs
+Reply:
+    Complex name editable in case we want to change it and then an unique accession which would be the actua identifier and</t>
       </text>
     </comment>
-    <comment ref="M69" authorId="5" shapeId="0" xr:uid="{2B9A8B6C-00AD-4E85-91E5-666B4DFA8621}">
+    <comment ref="M69" authorId="6" shapeId="0" xr:uid="{2B9A8B6C-00AD-4E85-91E5-666B4DFA8621}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -174,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="288">
   <si>
     <t>prot_seq</t>
   </si>
@@ -965,9 +999,6 @@
     <t>Normalisation_2</t>
   </si>
   <si>
-    <t>Essential_for_complex_assembly</t>
-  </si>
-  <si>
     <t>Normalisation_3</t>
   </si>
   <si>
@@ -1008,6 +1039,42 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>Shell Interactions</t>
+  </si>
+  <si>
+    <t>Core and Support Interactions</t>
+  </si>
+  <si>
+    <t>Essential_for_their_corresponding_complex_assembly</t>
+  </si>
+  <si>
+    <t>Essential for assembly of a BMC_complex_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Strategy define define complex firt, </t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>simulated</t>
+  </si>
+  <si>
+    <t>Modelled</t>
+  </si>
+  <si>
+    <t>true.false categories instead of column</t>
+  </si>
+  <si>
+    <t>accession_number</t>
+  </si>
+  <si>
+    <t>for prot gene and complex and it is sufficently unique</t>
+  </si>
+  <si>
+    <t>parent_sequence</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1297,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1440,6 +1507,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1601,7 +1680,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="6" applyFont="1"/>
@@ -1649,6 +1728,8 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="6" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1705,6 +1786,160 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>496094</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>168673</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>181429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E203E712-295A-DD9C-2684-EDCCC7B02198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2469130" y="5520814"/>
+          <a:ext cx="1645614" cy="3437222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>549189</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>188783</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>380400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9177DB-4476-F4BE-153E-BEC44BC89D44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14673648" y="9662297"/>
+          <a:ext cx="5048509" cy="1416123"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>446216</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>409735</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>129685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686FF060-B08C-F67A-D3EC-EAD9DA36F6EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19787973" y="9679459"/>
+          <a:ext cx="5180816" cy="1365361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2033,9 +2268,15 @@
   <threadedComment ref="AB6" dT="2025-05-13T14:16:04.33" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
     <text>do I want the origin organism for the modfied versions, I think it is useful information but may cause confusion</text>
   </threadedComment>
+  <threadedComment ref="AB6" dT="2025-06-05T13:25:48.06" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{0D0B161A-A123-4F95-A9AB-CD3E4830D839}" parentId="{718FA20F-218F-4912-8B43-B2DC1C016F9E}">
+    <text>If unchange sequence reasonable, when modifie no tax</text>
+  </threadedComment>
   <threadedComment ref="Y8" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
     <text xml:space="preserve">Would it be null as it comes from a modified version or would I want it still on comments?
 </text>
+  </threadedComment>
+  <threadedComment ref="Y8" dT="2025-06-05T13:27:42.91" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{EB39687E-8D8F-4849-93D8-51C19D17F88D}" parentId="{91933B1A-8BE8-4E5E-BEA5-DEE0A75A6C45}">
+    <text>fine</text>
   </threadedComment>
   <threadedComment ref="S19" dT="2025-05-13T14:10:47.92" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{9DB239A6-8497-4387-833D-57D2AED81F35}">
     <text xml:space="preserve">Would it be null as it comes from a modified version or would I want it still on comments?
@@ -2053,6 +2294,9 @@
   <threadedComment ref="N37" dT="2025-05-13T14:30:14.15" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{62240600-B1E7-44E6-B96A-5BEA743DB408}" parentId="{189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}">
     <text>KEGG: related genes, papers, function</text>
   </threadedComment>
+  <threadedComment ref="W38" dT="2025-06-05T13:30:03.87" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{DF0AE6F2-F317-4F6F-AF56-764C13C56519}">
+    <text>Dentifer for engineering change sequence that inmediately preceds it</text>
+  </threadedComment>
   <threadedComment ref="V39" dT="2025-06-03T11:12:56.45" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}">
     <text>Add condition that if origin true origin_cds null?</text>
   </threadedComment>
@@ -2068,15 +2312,36 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L31" dT="2025-06-03T14:49:46.42" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+  <threadedComment ref="F30" dT="2025-06-05T12:47:51.11" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{AEC729A6-7C26-49DC-9714-BAA59955DFAE}">
+    <text xml:space="preserve">Describe the complex in what type of interaction (beisbl ball example), Represent how individal members interact with each other. </text>
+  </threadedComment>
+  <threadedComment ref="F30" dT="2025-06-05T13:00:02.70" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{C53D3B0A-49C8-42F3-85E9-F138B066D2D5}" parentId="{AEC729A6-7C26-49DC-9714-BAA59955DFAE}">
+    <text xml:space="preserve">Have 2 queries when searching for information and remove repetition, also make interaction depending on complex </text>
+  </threadedComment>
+  <threadedComment ref="F30" dT="2025-06-05T13:00:53.00" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{54311013-2462-4651-BDDF-635EB0760EC8}" parentId="{AEC729A6-7C26-49DC-9714-BAA59955DFAE}">
+    <text xml:space="preserve"> </text>
+  </threadedComment>
+  <threadedComment ref="AB33" dT="2025-06-03T14:49:46.42" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
     <text xml:space="preserve">Unsure about this being clear enough, comment on native example
 </text>
   </threadedComment>
-  <threadedComment ref="F54" dT="2025-06-03T15:01:57.61" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
+  <threadedComment ref="AB33" dT="2025-06-04T14:54:18.45" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{FADD74A2-C4F7-4031-BF40-0842DB54FB71}" parentId="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+    <text>Pdu, HO compare and decide which one that gives me unique information.</text>
+  </threadedComment>
+  <threadedComment ref="AB33" dT="2025-06-04T14:56:41.60" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{4A26ADDB-4575-42FC-A8EC-11EC0E6259BF}" parentId="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+    <text>Definition of complex that reflects the differences so I have the categories and therefore I can put differences between pdue and eut</text>
+  </threadedComment>
+  <threadedComment ref="AB33" dT="2025-06-05T12:33:25.53" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{72E33364-B802-4848-A714-265F6F22D8D3}" parentId="{0F9AD2A1-2F87-43BD-9092-A77977442708}">
+    <text>Leave it aside for now and we can apply it later on</text>
+  </threadedComment>
+  <threadedComment ref="G54" dT="2025-06-03T15:01:57.61" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
     <text>I know what I want to do, but not sure how to sestablish nomenclature. As this is a if prot_id_1 interacts with prot_id_2 then I don’t need to add that prot_id_2 interacts with prot_id_1</text>
   </threadedComment>
-  <threadedComment ref="F54" dT="2025-06-03T15:09:03.87" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{84724DDB-1CFE-4133-88A1-3DDE10981BA8}" parentId="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
+  <threadedComment ref="G54" dT="2025-06-03T15:09:03.87" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{84724DDB-1CFE-4133-88A1-3DDE10981BA8}" parentId="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
     <text>Also this table is like apart from the others in the same that I think I don’t want it related to the complex as the porteins interacts with those, so I know that, that prot 1 interacts with 2 and 3, and I know what the complex is made of so if it has 2 but not 3 is quite obvious what is interacting. Does that make sense?</text>
+  </threadedComment>
+  <threadedComment ref="G54" dT="2025-06-05T10:27:06.94" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{88BA29C8-179A-4C17-9C7A-1F66353A136F}" parentId="{7B8A5F05-6DF0-48C3-91D3-B0B9253773C3}">
+    <text>Interactions 2 spearate categories? EP core and shell structure for assembly?</text>
   </threadedComment>
   <threadedComment ref="L54" dT="2025-06-03T14:49:46.42" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{EF411826-7395-4077-8E4B-D55F86DAD678}">
     <text xml:space="preserve">Unsure about this being clear enough, comment on native example
@@ -2091,6 +2356,9 @@
   <threadedComment ref="J69" dT="2025-06-03T15:12:28.86" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{237F9E53-A724-461A-9D97-96190E1F43BA}">
     <text>This is not needed for database is so I can make sense in my head with the names I give to things, or would it be helpful? Names may be repeated by type but I do use them for experimental purposes when naming constructs</text>
   </threadedComment>
+  <threadedComment ref="J69" dT="2025-06-05T13:15:46.47" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{4E2EF8B5-EEC3-4A9B-ABD7-6501461855AE}" parentId="{237F9E53-A724-461A-9D97-96190E1F43BA}">
+    <text>Complex name editable in case we want to change it and then an unique accession which would be the actua identifier and</text>
+  </threadedComment>
   <threadedComment ref="M69" dT="2025-06-03T15:22:08.03" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{2B9A8B6C-00AD-4E85-91E5-666B4DFA8621}">
     <text>What if I want to refer to a paper where they test the activty? Should I do it like with external links in prot?</text>
   </threadedComment>
@@ -2104,8 +2372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783CC8DE-7F76-644C-B681-A92CC700BEB1}">
   <dimension ref="A1:AO84"/>
   <sheetViews>
-    <sheetView topLeftCell="H25" zoomScale="62" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AA50" sqref="AA50"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="30" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -4207,11 +4475,11 @@
       <c r="U38" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="V38" s="1" t="s">
+      <c r="V38" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="W38" s="1" t="s">
-        <v>131</v>
+      <c r="W38" s="9" t="s">
+        <v>287</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>63</v>
@@ -4269,7 +4537,7 @@
       <c r="U39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V39" s="1" t="b">
+      <c r="V39" s="9" t="b">
         <v>1</v>
       </c>
       <c r="W39" s="28" t="s">
@@ -4319,7 +4587,7 @@
       <c r="U40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V40" s="1" t="b">
+      <c r="V40" s="9" t="b">
         <v>1</v>
       </c>
       <c r="W40" s="28" t="s">
@@ -4369,7 +4637,7 @@
       <c r="U41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V41" s="1" t="b">
+      <c r="V41" s="9" t="b">
         <v>1</v>
       </c>
       <c r="W41" s="28" t="s">
@@ -4425,7 +4693,7 @@
       <c r="U42" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="V42" s="1" t="b">
+      <c r="V42" s="9" t="b">
         <v>1</v>
       </c>
       <c r="W42" s="28" t="s">
@@ -4487,7 +4755,7 @@
       <c r="U43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="V43" s="1" t="b">
+      <c r="V43" s="9" t="b">
         <v>0</v>
       </c>
       <c r="W43" s="28">
@@ -4544,12 +4812,12 @@
         <v>6</v>
       </c>
       <c r="T44" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="V44" s="1" t="b">
+      <c r="V44" s="9" t="b">
         <v>0</v>
       </c>
       <c r="W44" s="28">
@@ -4605,7 +4873,7 @@
       <c r="U45" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="V45" s="1" t="b">
+      <c r="V45" s="9" t="b">
         <v>0</v>
       </c>
       <c r="W45" s="28">
@@ -5442,10 +5710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B80FE9-C3C3-4D64-8637-D3E1F6A95FD2}">
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView topLeftCell="A25" zoomScale="37" workbookViewId="0">
+      <selection activeCell="R71" sqref="R71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -5562,13 +5830,13 @@
         <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>235</v>
@@ -5577,7 +5845,7 @@
         <v>235</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>216</v>
@@ -5639,10 +5907,10 @@
         <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>40</v>
@@ -5651,7 +5919,7 @@
         <v>235</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>40</v>
@@ -5716,10 +5984,10 @@
         <v>40</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>40</v>
@@ -5728,7 +5996,7 @@
         <v>235</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>40</v>
@@ -5793,10 +6061,10 @@
         <v>40</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>40</v>
@@ -5805,7 +6073,7 @@
         <v>235</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>40</v>
@@ -5870,10 +6138,10 @@
         <v>227</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>40</v>
@@ -5882,7 +6150,7 @@
         <v>235</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>40</v>
@@ -5947,10 +6215,10 @@
         <v>40</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>40</v>
@@ -5959,7 +6227,7 @@
         <v>235</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>40</v>
@@ -6024,7 +6292,7 @@
         <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>40</v>
@@ -6033,7 +6301,7 @@
         <v>40</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>40</v>
@@ -6226,7 +6494,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -6261,7 +6529,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -6296,7 +6564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -6331,7 +6599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>7</v>
       </c>
@@ -6366,7 +6634,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="L21" s="1">
         <v>1</v>
       </c>
@@ -6377,7 +6645,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>249</v>
       </c>
@@ -6406,12 +6674,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>235</v>
@@ -6435,12 +6703,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>235</v>
@@ -6464,15 +6732,15 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>216</v>
@@ -6493,7 +6761,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="L26" s="1">
         <v>6</v>
       </c>
@@ -6504,7 +6772,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="L27" s="1">
         <v>7</v>
       </c>
@@ -6515,480 +6783,631 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I30" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="I30" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>201</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="H31" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="I31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E32" s="1">
-        <v>1</v>
+      <c r="D32" s="33" t="s">
+        <v>215</v>
       </c>
       <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
         <v>3</v>
       </c>
       <c r="I32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="K32" s="1">
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1">
         <v>23453</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A33" s="1">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>203</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E33" s="1">
-        <v>2</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="D33" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="G33" s="32">
         <v>1</v>
       </c>
       <c r="I33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" s="1">
-        <v>2</v>
-      </c>
-      <c r="K33" s="1">
+        <v>5</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2</v>
+      </c>
+      <c r="P33" s="1">
         <v>45387</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A34" s="1">
-        <v>3</v>
-      </c>
+      <c r="V33" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="W33" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z33" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA33" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB33" s="34" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
         <v>204</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E34" s="32">
-        <v>3</v>
-      </c>
-      <c r="F34" s="32">
-        <v>1</v>
-      </c>
-      <c r="I34" s="1">
-        <v>2</v>
-      </c>
-      <c r="J34" s="1">
-        <v>2</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="D34" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="32">
+        <v>5</v>
+      </c>
+      <c r="J34" s="32">
+        <v>2</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2</v>
+      </c>
+      <c r="O34" s="1">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A35" s="1">
-        <v>4</v>
-      </c>
+      <c r="V34" s="34">
+        <v>1</v>
+      </c>
+      <c r="W34" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z34" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="34">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="1">
-        <v>4</v>
+      <c r="D35" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="I35" s="1">
-        <v>3</v>
-      </c>
-      <c r="J35" s="1">
-        <v>2</v>
-      </c>
-      <c r="K35" s="1">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="32">
+        <v>1</v>
+      </c>
+      <c r="J35" s="32">
+        <v>2</v>
+      </c>
+      <c r="N35" s="1">
+        <v>3</v>
+      </c>
+      <c r="O35" s="1">
+        <v>2</v>
+      </c>
+      <c r="P35" s="1">
         <v>30000</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="V35" s="34">
+        <v>2</v>
+      </c>
+      <c r="W35" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z35" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A36" s="1">
-        <v>5</v>
-      </c>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>206</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E36" s="1">
+      <c r="D36" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="1">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1">
         <v>5</v>
       </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="I36" s="1">
+      <c r="N36" s="1">
         <v>4</v>
       </c>
-      <c r="J36" s="1">
-        <v>2</v>
-      </c>
-      <c r="K36" s="1">
+      <c r="O36" s="1">
+        <v>2</v>
+      </c>
+      <c r="P36" s="1">
         <v>70</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A37" s="1">
-        <v>6</v>
-      </c>
+      <c r="V36" s="34">
+        <v>3</v>
+      </c>
+      <c r="W36" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z36" s="34">
+        <v>2</v>
+      </c>
+      <c r="AA36" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB36" s="34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B37" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E37" s="1">
-        <v>6</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="D37" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="32">
+        <v>1</v>
+      </c>
+      <c r="G37" s="32">
+        <v>4</v>
+      </c>
+      <c r="N37" s="1">
         <v>5</v>
       </c>
-      <c r="I37" s="1">
-        <v>5</v>
-      </c>
-      <c r="J37" s="1">
-        <v>2</v>
-      </c>
-      <c r="K37" s="1">
+      <c r="O37" s="1">
+        <v>2</v>
+      </c>
+      <c r="P37" s="1">
         <v>30</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="V37" s="34">
+        <v>4</v>
+      </c>
+      <c r="W37" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z37" s="34">
+        <v>3</v>
+      </c>
+      <c r="AA37" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB37" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A38" s="1">
-        <v>7</v>
-      </c>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B38" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E38" s="32">
-        <v>1</v>
-      </c>
-      <c r="F38" s="32">
+      <c r="D38" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1">
+        <v>5</v>
+      </c>
+      <c r="N38" s="1">
+        <v>6</v>
+      </c>
+      <c r="O38" s="1">
+        <v>2</v>
+      </c>
+      <c r="P38" s="1">
+        <v>200</v>
+      </c>
+      <c r="V38" s="34">
+        <v>5</v>
+      </c>
+      <c r="W38" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z38" s="34">
         <v>4</v>
       </c>
-      <c r="I38" s="1">
+      <c r="AA38" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB38" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="F39" s="1">
+        <v>4</v>
+      </c>
+      <c r="G39" s="1">
+        <v>5</v>
+      </c>
+      <c r="N39" s="1">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1">
+        <v>3</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V39" s="34">
         <v>6</v>
       </c>
-      <c r="J38" s="1">
-        <v>2</v>
-      </c>
-      <c r="K38" s="1">
-        <v>200</v>
-      </c>
-      <c r="L38" s="1" t="s">
+      <c r="W39" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z39" s="34">
+        <v>5</v>
+      </c>
+      <c r="AA39" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB39" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E39" s="1">
-        <v>2</v>
-      </c>
-      <c r="F39" s="1">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="F40" s="32">
         <v>5</v>
       </c>
-      <c r="I39" s="1">
-        <v>1</v>
-      </c>
-      <c r="J39" s="1">
-        <v>3</v>
-      </c>
-      <c r="K39" s="1" t="s">
+      <c r="G40" s="32">
+        <v>3</v>
+      </c>
+      <c r="N40" s="1">
+        <v>3</v>
+      </c>
+      <c r="O40" s="1">
+        <v>3</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="V40" s="34">
+        <v>7</v>
+      </c>
+      <c r="W40" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z40" s="34">
+        <v>6</v>
+      </c>
+      <c r="AA40" s="34">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E40" s="1">
-        <v>3</v>
-      </c>
-      <c r="F40" s="1">
+    <row r="41" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="F41" s="32">
+        <v>1</v>
+      </c>
+      <c r="G41" s="32">
         <v>5</v>
       </c>
-      <c r="I40" s="1">
-        <v>3</v>
-      </c>
-      <c r="J40" s="1">
-        <v>3</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="N41" s="1">
+        <v>4</v>
+      </c>
+      <c r="O41" s="1">
+        <v>3</v>
+      </c>
+      <c r="P41" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="Z41" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB41" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E41" s="1">
-        <v>4</v>
-      </c>
-      <c r="F41" s="1">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="F42" s="1">
+        <v>3</v>
+      </c>
+      <c r="G42" s="1">
+        <v>6</v>
+      </c>
+      <c r="N42" s="1">
         <v>5</v>
       </c>
-      <c r="I41" s="1">
-        <v>4</v>
-      </c>
-      <c r="J41" s="1">
-        <v>3</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="O42" s="1">
+        <v>3</v>
+      </c>
+      <c r="P42" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="Z42" s="34">
+        <v>3</v>
+      </c>
+      <c r="AA42" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB42" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E42" s="32">
-        <v>5</v>
-      </c>
-      <c r="F42" s="32">
-        <v>3</v>
-      </c>
-      <c r="I42" s="1">
-        <v>5</v>
-      </c>
-      <c r="J42" s="1">
-        <v>3</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E43" s="32">
-        <v>1</v>
-      </c>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.4">
       <c r="F43" s="32">
         <v>5</v>
       </c>
-      <c r="I43" s="1">
+      <c r="G43" s="32">
         <v>6</v>
       </c>
-      <c r="J43" s="1">
-        <v>3</v>
-      </c>
-      <c r="K43" s="1" t="s">
+      <c r="N43" s="1">
+        <v>6</v>
+      </c>
+      <c r="O43" s="1">
+        <v>3</v>
+      </c>
+      <c r="P43" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="Z43" s="34">
+        <v>4</v>
+      </c>
+      <c r="AA43" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB43" s="34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E44" s="1">
-        <v>3</v>
-      </c>
-      <c r="F44" s="1">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="N44" s="1">
+        <v>7</v>
+      </c>
+      <c r="O44" s="1">
+        <v>3</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="Z44" s="34">
+        <v>5</v>
+      </c>
+      <c r="AA44" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB44" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="Z45" s="34">
         <v>6</v>
       </c>
-      <c r="I44" s="1">
+      <c r="AA45" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB45" s="34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="N46" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z46" s="34">
         <v>7</v>
       </c>
-      <c r="J44" s="1">
-        <v>3</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="L44" s="1" t="s">
+      <c r="AA46" s="34">
+        <v>3</v>
+      </c>
+      <c r="AB46" s="34" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E45" s="32">
-        <v>5</v>
-      </c>
-      <c r="F45" s="32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="E46" s="32">
-        <v>5</v>
-      </c>
-      <c r="F46" s="32">
-        <v>2</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1" t="s">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="N47" s="1">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="N48" s="1">
+        <v>2</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="P48" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="Q48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="R48" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M47" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="I48" s="1">
-        <v>2</v>
-      </c>
-      <c r="J48" s="1" t="s">
+      <c r="S48" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="N49" s="1">
+        <v>3</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="M48" s="1" t="s">
+      <c r="P49" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q49" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="N48" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="I49" s="1">
-        <v>3</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="L49" s="1" t="s">
+      <c r="R49" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="N49" s="1" t="s">
+      <c r="S49" s="1" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>264</v>
+      <c r="F53" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>257</v>
@@ -7005,11 +7424,14 @@
       <c r="C54" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="D54" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>196</v>
@@ -7021,7 +7443,7 @@
         <v>197</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.4">
@@ -7034,10 +7456,13 @@
       <c r="C55" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E55" s="1">
-        <v>1</v>
+      <c r="D55" s="33" t="s">
+        <v>215</v>
       </c>
       <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
         <v>3</v>
       </c>
       <c r="I55" s="1">
@@ -7063,10 +7488,13 @@
       <c r="C56" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E56" s="1">
-        <v>2</v>
+      <c r="D56" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="F56" s="1">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1">
         <v>1</v>
       </c>
       <c r="I56" s="1">
@@ -7092,10 +7520,13 @@
       <c r="C57" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E57" s="1">
+      <c r="D57" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F57" s="1">
         <v>4</v>
       </c>
-      <c r="F57" s="1">
+      <c r="G57" s="1">
         <v>1</v>
       </c>
       <c r="I57" s="1">
@@ -7121,10 +7552,13 @@
       <c r="C58" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E58" s="1">
+      <c r="D58" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F58" s="1">
         <v>5</v>
       </c>
-      <c r="F58" s="1">
+      <c r="G58" s="1">
         <v>1</v>
       </c>
       <c r="I58" s="1">
@@ -7150,10 +7584,13 @@
       <c r="C59" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E59" s="1">
+      <c r="D59" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F59" s="1">
         <v>6</v>
       </c>
-      <c r="F59" s="1">
+      <c r="G59" s="1">
         <v>5</v>
       </c>
       <c r="I59" s="1">
@@ -7169,7 +7606,7 @@
         <v>215</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.4">
@@ -7182,10 +7619,13 @@
       <c r="C60" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E60" s="1">
-        <v>2</v>
+      <c r="D60" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="F60" s="1">
+        <v>2</v>
+      </c>
+      <c r="G60" s="1">
         <v>5</v>
       </c>
       <c r="I60" s="1">
@@ -7211,10 +7651,13 @@
       <c r="C61" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E61" s="1">
-        <v>3</v>
+      <c r="D61" s="33" t="s">
+        <v>216</v>
       </c>
       <c r="F61" s="1">
+        <v>3</v>
+      </c>
+      <c r="G61" s="1">
         <v>5</v>
       </c>
       <c r="I61" s="1">
@@ -7233,17 +7676,17 @@
         <v>200</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S61" s="6" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="E62" s="1">
+      <c r="F62" s="1">
         <v>4</v>
       </c>
-      <c r="F62" s="1">
+      <c r="G62" s="1">
         <v>5</v>
       </c>
       <c r="I62" s="1">
@@ -7262,17 +7705,17 @@
         <v>19</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S62" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="E63" s="1">
-        <v>3</v>
-      </c>
       <c r="F63" s="1">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1">
         <v>6</v>
       </c>
       <c r="I63" s="1">
@@ -7291,7 +7734,7 @@
         <v>255</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.4">
@@ -7311,10 +7754,10 @@
         <v>246</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="65" spans="9:14" x14ac:dyDescent="0.4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="6:18" x14ac:dyDescent="0.4">
       <c r="I65" s="1">
         <v>5</v>
       </c>
@@ -7327,8 +7770,17 @@
       <c r="L65" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="66" spans="9:14" x14ac:dyDescent="0.4">
+      <c r="O65" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="P65" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="6:18" x14ac:dyDescent="0.4">
+      <c r="F66" s="33" t="s">
+        <v>277</v>
+      </c>
       <c r="I66" s="1">
         <v>6</v>
       </c>
@@ -7341,8 +7793,17 @@
       <c r="L66" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="67" spans="9:14" x14ac:dyDescent="0.4">
+      <c r="O66" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="67" spans="6:18" x14ac:dyDescent="0.4">
+      <c r="F67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I67" s="1">
         <v>7</v>
       </c>
@@ -7356,7 +7817,21 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="9:14" x14ac:dyDescent="0.4">
+    <row r="68" spans="6:18" x14ac:dyDescent="0.4">
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="6:18" x14ac:dyDescent="0.4">
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
+      <c r="G69" s="1">
+        <v>5</v>
+      </c>
       <c r="I69" s="1" t="s">
         <v>249</v>
       </c>
@@ -7375,13 +7850,16 @@
       <c r="N69" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="70" spans="9:14" x14ac:dyDescent="0.4">
+      <c r="O69" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="70" spans="6:18" x14ac:dyDescent="0.4">
       <c r="I70" s="1">
         <v>1</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>235</v>
@@ -7395,13 +7873,16 @@
       <c r="N70" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="71" spans="9:14" x14ac:dyDescent="0.4">
+      <c r="R70" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="71" spans="6:18" x14ac:dyDescent="0.4">
       <c r="I71" s="1">
         <v>2</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>235</v>
@@ -7416,15 +7897,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="9:14" x14ac:dyDescent="0.4">
+    <row r="72" spans="6:18" x14ac:dyDescent="0.4">
       <c r="I72" s="1">
         <v>3</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>216</v>
@@ -7439,7 +7920,8 @@
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updating db.py to reflect the changes made in normalisation. Process ongoing. The update is being performed on the file db-new.py
</commit_message>
<xml_diff>
--- a/docs/normalisation_thoughts/normalisation_database.xlsx
+++ b/docs/normalisation_thoughts/normalisation_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monserrj\1.BMC\BMC-database-1\docs\normalisation_thoughts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347A3A6-172E-4FA9-ACCC-64077C8034AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468618E7-D782-4F86-8B65-B14C5F7463A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
   </bookViews>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="288">
   <si>
     <t>prot_seq</t>
   </si>
@@ -1081,7 +1081,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1283,18 +1283,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -2372,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783CC8DE-7F76-644C-B681-A92CC700BEB1}">
   <dimension ref="A1:AO84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="30" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView tabSelected="1" topLeftCell="I27" zoomScale="48" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -5048,9 +5036,7 @@
       <c r="L50" s="1">
         <v>3</v>
       </c>
-      <c r="S50" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="S50" s="15"/>
       <c r="T50" s="1" t="s">
         <v>63</v>
       </c>
@@ -5089,9 +5075,7 @@
       <c r="L51" s="1">
         <v>3</v>
       </c>
-      <c r="S51" s="1">
-        <v>1</v>
-      </c>
+      <c r="S51" s="15"/>
       <c r="T51" s="1">
         <v>1</v>
       </c>
@@ -5131,9 +5115,7 @@
       <c r="L52" s="1">
         <v>4</v>
       </c>
-      <c r="S52" s="1">
-        <v>2</v>
-      </c>
+      <c r="S52" s="15"/>
       <c r="T52" s="1">
         <v>2</v>
       </c>
@@ -5166,9 +5148,7 @@
       <c r="P53" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="S53" s="1">
-        <v>3</v>
-      </c>
+      <c r="S53" s="15"/>
       <c r="T53" s="1">
         <v>3</v>
       </c>
@@ -5200,9 +5180,7 @@
         <v>115</v>
       </c>
       <c r="P54" s="6"/>
-      <c r="S54" s="1">
-        <v>4</v>
-      </c>
+      <c r="S54" s="15"/>
       <c r="T54" s="1">
         <v>4</v>
       </c>
@@ -5233,9 +5211,7 @@
         <v>116</v>
       </c>
       <c r="P55" s="6"/>
-      <c r="S55" s="1">
-        <v>5</v>
-      </c>
+      <c r="S55" s="15"/>
       <c r="T55" s="1">
         <v>5</v>
       </c>
@@ -5266,9 +5242,7 @@
         <v>117</v>
       </c>
       <c r="P56" s="6"/>
-      <c r="S56" s="1">
-        <v>6</v>
-      </c>
+      <c r="S56" s="15"/>
       <c r="T56" s="1">
         <v>6</v>
       </c>
@@ -5301,9 +5275,7 @@
       <c r="P57" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="S57" s="1">
-        <v>7</v>
-      </c>
+      <c r="S57" s="15"/>
       <c r="T57" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
update of excels for data interrogation - only half (those with UP)
</commit_message>
<xml_diff>
--- a/docs/normalisation_thoughts/normalisation_database.xlsx
+++ b/docs/normalisation_thoughts/normalisation_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monserrj\1.BMC\BMC-database-1\docs\normalisation_thoughts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monserrj\BMC-database\docs\normalisation_thoughts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468618E7-D782-4F86-8B65-B14C5F7463A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C10FE36-B81A-43B9-8BE1-4C08CB906F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E47BD96-BEA0-4242-8AB7-AE769A8DB2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="prot_data_minimal_correct" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="experiments(postponed)" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -30,7 +31,6 @@
     <author>tc={189EE3C0-D22E-4F5C-A8F1-4AE828A7C9E4}</author>
     <author>tc={DF0AE6F2-F317-4F6F-AF56-764C13C56519}</author>
     <author>tc={03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}</author>
-    <author>tc={60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}</author>
     <author>tc={8225B6DE-5319-428D-90CE-8EDEFF5C5865}</author>
   </authors>
   <commentList>
@@ -93,15 +93,7 @@
     Add condition that if origin true origin_cds null?</t>
       </text>
     </comment>
-    <comment ref="P60" authorId="6" shapeId="0" xr:uid="{60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Check this change</t>
-      </text>
-    </comment>
-    <comment ref="N65" authorId="7" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
+    <comment ref="N65" authorId="6" shapeId="0" xr:uid="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -208,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="290">
   <si>
     <t>prot_seq</t>
   </si>
@@ -546,9 +538,6 @@
     <t>ATGAGCAGCAATGAGCTGGTTGATCAGATCATGGCGCAGGTGATTGCTCGCGTGGCAACGCCGGAACAGCAGGCTATCCCTGAAAATAATCCTCCAACACGAGAAACGGCTATGGCAGAGAAAAGCTGCAGTTTAACGGAGTTTGTCGGTACTGCGATTGGCGACACCGTCGGTCTGGTAATCGCCAACGTGGACAGCGCCCTACTGGACGCAATGAAACTTGAAAAACGGTATCGCTCCATTGGCATCCTTGGCGCGCGTACTGGTGCAGGCCCGCACATCATGGCCGCAGATGAAGCGGTAAAAGCCACCAATACTGAAGTCGTCAGTATTGAGTTGCCACGTGATACCAAAGGCGGCGCGGGTCACGGTTCGCTGATTATTCTCGGCGGCAACGATGTTTCCGACGTGAAACGCGGAATTGAGGTTGCGCTGAAAGAACTGGATCGCACCTTTGGCGATGTGTATGCCAACGAAGCCGGTCACATCGAGATGCAATACACCGCACGCGCCAGCTACGCGCTGGAAAAAGCCTTTGGTGCACCGATTGGCCGTGCCTGTGGCGTGATCGTCGGCGCGCCGGCATCCGTTGGTGTCCTGATGGCTGATACTGCGCTGAAATCCGCCAACGTGGAAGTTGTGGCCTACAGCTCCCCTGCCCATGGCACCAGCTTCAGTAACGAAGCCATTCTGGTCATTTCAGGCGATTCCGGCGCTGTGCGTCAGGCCGTTATCTCCGCCCGCGAAATCGGTAAAACCGTACTCGGGACCCTCGGCTCAGAACCGAAAAACGATCGTCCGTCCTACATCTGA</t>
   </si>
   <si>
-    <t>optimised</t>
-  </si>
-  <si>
     <t>ATAGAAGACGCAATGGACTCACAATTAGTTCTGAGCTTGAAACTGAACCCTAGCTTTACACCTCTCTCCCCATTGTTCCCTTTCACTCCATGCTCAAGTTTTTCCCCTAGCCTGCGTTTTAGCAGCTGTTATTCCCGTCGTCTGTATTCCCCAGTTACAGTGTACGCTGCAAAAAAATTGAGCCATAAAATTAGCTCCGAGTTCGATGATCGTAGCTCAAACGAGCTTGTGGACCAGATTATGGCTCAAGTGATTGCCCGTGTCGCAACTCCAGAACAGCAGGCTATCCCTGAGAATAACCCACCTACACGTGAGACAGCCATGGCCGAGAAATCCTGTTCTTTGACAGAGTTCGTTGGCACCGCTATTGGAGATACCGTTGGTCTGGTGATCGCTAACGTAGACAGTGCTCTGCTCGATGCTATGAAACTTGAGAAACGTTATCGTAGCATCGGAATTCTCGGCGCACGTACAGGAGCCGGTCCACACATTATGGCCGCCGATGAAGCTGTAAAAGCAACTAATACCGAAGTTGTTAGTATTGAACTTCCACGTGACACTAAAGGCGGAGCCGGACACGGGTCATTGATCATCCTGGGTGGCAATGACGTGAGCGATGTTAAGCGTGGCATTGAGGTGGCCCTTAAGGAATTGGACCGTACTTTCGGTGATGTATACGCTAATGAAGCCGGCCATATCGAGATGCAGTATACCGCTCGTGCTTCTTACGCATTGGAAAAGGCTTTTGGGGCCCCTATTGGTCGTGCTTGTGGCGTGATCGTAGGTGCTCCAGCTAGTGTGGGCGTCCTGATGGCAGATACAGCTTTAAAAAGCGCAAATGTAGAAGTTGTGGCTTACTCTTCCCCAGCTCACGGCACATCATTTAGTAACGAAGCCATTCTGGTGATTTCAGGGGATTCTGGGGCTGTTCGTCAAGCTGTAATTTCAGCTCGTGAGATCGGTAAAACAGTGCTTGGTACTCTGGGCTCCGAGCCAAAGAACGACCGTCCATCTTATATCTGAGCTTCGGTCTTCATA</t>
   </si>
   <si>
@@ -579,12 +568,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Coding sequence from the original genome.</t>
-  </si>
-  <si>
-    <t>Codon optimised for heterologous expression (e.g., in E. coli, yeast).</t>
-  </si>
-  <si>
     <t>truncated</t>
   </si>
   <si>
@@ -609,18 +592,9 @@
     <t>origin_cds</t>
   </si>
   <si>
-    <t>modified</t>
-  </si>
-  <si>
-    <t>Coding sequence modified for different purposes</t>
-  </si>
-  <si>
     <t>modification_type</t>
   </si>
   <si>
-    <t>cds_type</t>
-  </si>
-  <si>
     <t>domesticated</t>
   </si>
   <si>
@@ -774,9 +748,6 @@
     <t>Native?</t>
   </si>
   <si>
-    <t>TRUE/FALSE -- if false modification type</t>
-  </si>
-  <si>
     <t>PCR modified to remove IRB</t>
   </si>
   <si>
@@ -1075,6 +1046,33 @@
   </si>
   <si>
     <t>parent_sequence</t>
+  </si>
+  <si>
+    <t>comple_source</t>
+  </si>
+  <si>
+    <t>Native complex, observed in nature (full operon)</t>
+  </si>
+  <si>
+    <t>Laboratory engineered for specific reasons</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>Predicted with alphaphold and other tools</t>
+  </si>
+  <si>
+    <t>Theoretical</t>
+  </si>
+  <si>
+    <t>Nor designed in silico nor testing in vivo, but theoretical concept that ust be further studied to see if possible?</t>
+  </si>
+  <si>
+    <t>extended</t>
+  </si>
+  <si>
+    <t>Lengthened vrsions of the coding sequence</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1491,12 +1489,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1668,7 +1660,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="6" applyFont="1"/>
@@ -1714,10 +1706,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="6" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" xfId="6" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2288,9 +2279,6 @@
   <threadedComment ref="V39" dT="2025-06-03T11:12:56.45" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{03BD69D8-F0A9-45A3-9FD4-7C3445D4EB56}">
     <text>Add condition that if origin true origin_cds null?</text>
   </threadedComment>
-  <threadedComment ref="P60" dT="2025-06-03T11:18:26.37" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{60FEA9FE-3368-4F6C-BF6E-52FC7827BA7D}">
-    <text>Check this change</text>
-  </threadedComment>
   <threadedComment ref="N65" dT="2025-05-13T14:08:36.10" personId="{2760B052-618A-4E7B-8D20-048EA6CB7516}" id="{8225B6DE-5319-428D-90CE-8EDEFF5C5865}">
     <text xml:space="preserve">Unsure as you can make many modifications to the same DNA sequence if I can add them all to the same protein (maybe like the pdb?)
 </text>
@@ -2358,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783CC8DE-7F76-644C-B681-A92CC700BEB1}">
-  <dimension ref="A1:AO84"/>
+  <dimension ref="A1:AO85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I27" zoomScale="48" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54:O57"/>
+    <sheetView tabSelected="1" topLeftCell="H46" zoomScale="48" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q64" sqref="Q64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2383,52 +2371,52 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" t="s">
         <v>157</v>
       </c>
-      <c r="J1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O1" t="s">
-        <v>163</v>
-      </c>
       <c r="P1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="Q1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="R1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>3</v>
@@ -2437,25 +2425,25 @@
         <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>6</v>
@@ -2464,7 +2452,7 @@
         <v>7</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AE1" t="s">
         <v>8</v>
@@ -2476,28 +2464,28 @@
         <v>10</v>
       </c>
       <c r="AH1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="AI1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AJ1" t="s">
         <v>11</v>
       </c>
       <c r="AK1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AL1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AM1" t="s">
         <v>12</v>
       </c>
       <c r="AN1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AO1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.4">
@@ -2517,28 +2505,28 @@
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>40</v>
@@ -2586,7 +2574,7 @@
         <v>502025</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>70</v>
@@ -2642,28 +2630,28 @@
         <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>40</v>
@@ -2711,7 +2699,7 @@
         <v>99287</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>70</v>
@@ -2767,37 +2755,37 @@
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Q4" s="1" t="b">
         <v>0</v>
@@ -2836,7 +2824,7 @@
         <v>546</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>70</v>
@@ -2892,28 +2880,28 @@
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>40</v>
@@ -2961,7 +2949,7 @@
         <v>99287</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>70</v>
@@ -3017,37 +3005,37 @@
         <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Q6" s="1" t="b">
         <v>1</v>
@@ -3086,7 +3074,7 @@
         <v>546</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>70</v>
@@ -3142,37 +3130,37 @@
         <v>109</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Q7" s="1" t="b">
         <v>1</v>
@@ -3190,28 +3178,28 @@
         <v>0</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W7" s="1">
         <v>4</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="AB7" s="1">
         <v>546</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD7" s="1" t="s">
         <v>70</v>
@@ -3267,37 +3255,37 @@
         <v>109</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Q8" s="1" t="b">
         <v>1</v>
@@ -3315,26 +3303,26 @@
         <v>0</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W8" s="1">
         <v>5</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1">
         <v>546</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>70</v>
@@ -3390,28 +3378,28 @@
         <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>40</v>
@@ -3438,28 +3426,28 @@
         <v>0</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="W9" s="1">
         <v>2</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="AB9" s="1">
         <v>99287</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AD9" s="1" t="s">
         <v>70</v>
@@ -3544,19 +3532,19 @@
         <v>65</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.4">
@@ -3570,7 +3558,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -3823,22 +3811,22 @@
         <v>4</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S18" s="20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="T18" s="21" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="U18" s="21" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="V18" s="28">
         <v>4</v>
@@ -3868,19 +3856,19 @@
         <v>4</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="T19" s="21" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="U19" s="21" t="s">
         <v>40</v>
@@ -3920,22 +3908,22 @@
         <v>2</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="Q20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S20" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="T20" s="21" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="U20" s="21" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="V20" s="28">
         <v>2</v>
@@ -4136,7 +4124,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="1">
         <v>13</v>
@@ -4246,7 +4234,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="D29" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G29" s="1">
         <v>16</v>
@@ -4281,10 +4269,10 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.4">
       <c r="D30" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G30" s="1">
         <v>17</v>
@@ -4376,7 +4364,7 @@
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.4">
@@ -4410,14 +4398,14 @@
         <v>44</v>
       </c>
       <c r="N37" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U37" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V37" s="2"/>
       <c r="Y37" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.4">
@@ -4434,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>45</v>
@@ -4443,7 +4431,7 @@
         <v>42</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>47</v>
@@ -4467,13 +4455,13 @@
         <v>65</v>
       </c>
       <c r="W38" s="9" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>63</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.4">
@@ -4496,7 +4484,7 @@
         <v>79</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="K39" s="1">
         <v>1</v>
@@ -4741,7 +4729,7 @@
         <v>4</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V43" s="9" t="b">
         <v>0</v>
@@ -4803,7 +4791,7 @@
         <v>5</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V44" s="9" t="b">
         <v>0</v>
@@ -4844,10 +4832,10 @@
         <v>7</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>82</v>
@@ -4859,7 +4847,7 @@
         <v>2</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="V45" s="9" t="b">
         <v>0</v>
@@ -4900,16 +4888,16 @@
         <v>8</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>82</v>
       </c>
       <c r="AA46" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.4">
@@ -4941,13 +4929,13 @@
         <v>2</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AA47" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.4">
@@ -4961,7 +4949,7 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G48" s="1">
         <v>9</v>
@@ -4982,10 +4970,10 @@
         <v>1</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AA48" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.4">
@@ -5011,15 +4999,15 @@
         <v>2</v>
       </c>
       <c r="Z49" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.4">
       <c r="D50" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1">
         <v>11</v>
@@ -5047,18 +5035,18 @@
         <v>3</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AA50" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.4">
       <c r="D51" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G51" s="1">
         <v>12</v>
@@ -5086,10 +5074,10 @@
         <v>4</v>
       </c>
       <c r="Z51" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AA51" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.4">
@@ -5143,10 +5131,10 @@
         <v>80</v>
       </c>
       <c r="O53" s="30" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="P53" s="30" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="S53" s="15"/>
       <c r="T53" s="1">
@@ -5177,7 +5165,7 @@
         <v>81</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P54" s="6"/>
       <c r="S54" s="15"/>
@@ -5193,7 +5181,7 @@
         <v>16</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I55" s="1">
         <v>7</v>
@@ -5208,7 +5196,7 @@
         <v>82</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P55" s="6"/>
       <c r="S55" s="15"/>
@@ -5224,7 +5212,7 @@
         <v>17</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I56" s="1">
         <v>7</v>
@@ -5239,7 +5227,7 @@
         <v>83</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P56" s="6"/>
       <c r="S56" s="15"/>
@@ -5255,7 +5243,7 @@
         <v>18</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I57" s="1">
         <v>7</v>
@@ -5270,10 +5258,10 @@
         <v>84</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="S57" s="15"/>
       <c r="T57" s="1">
@@ -5288,7 +5276,7 @@
         <v>19</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I58" s="1">
         <v>8</v>
@@ -5305,7 +5293,7 @@
         <v>20</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I59" s="1">
         <v>8</v>
@@ -5322,7 +5310,7 @@
         <v>21</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I60" s="1">
         <v>7</v>
@@ -5334,16 +5322,6 @@
       <c r="L60" s="1">
         <v>2</v>
       </c>
-      <c r="N60" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="O60" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="P60" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q60" s="31"/>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.4">
       <c r="G61" s="1">
@@ -5361,12 +5339,6 @@
       <c r="L61" s="1">
         <v>3</v>
       </c>
-      <c r="N61" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="O61" s="27" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.4">
       <c r="G62" s="1">
@@ -5384,12 +5356,6 @@
       <c r="L62" s="1">
         <v>4</v>
       </c>
-      <c r="N62" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="O62" s="27" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.4">
       <c r="G63" s="1">
@@ -5406,12 +5372,6 @@
       </c>
       <c r="L63" s="1">
         <v>3</v>
-      </c>
-      <c r="N63" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="O63" s="27" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.4">
@@ -5431,10 +5391,10 @@
       <c r="J65" s="15"/>
       <c r="K65" s="15"/>
       <c r="N65" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="O65" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.4">
@@ -5442,20 +5402,20 @@
       <c r="J66" s="15"/>
       <c r="K66" s="15"/>
       <c r="N66" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O66" s="18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.4">
       <c r="G67" s="15"/>
       <c r="J67" s="15"/>
       <c r="N67" s="17" t="s">
-        <v>125</v>
+        <v>288</v>
       </c>
       <c r="O67" s="18" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.4">
@@ -5463,10 +5423,10 @@
       <c r="H68" s="15"/>
       <c r="J68" s="15"/>
       <c r="N68" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="O68" s="18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.4">
@@ -5477,10 +5437,10 @@
       <c r="G69" s="15"/>
       <c r="J69" s="15"/>
       <c r="N69" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="O69" s="18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.4">
@@ -5491,10 +5451,10 @@
       <c r="G70" s="12"/>
       <c r="J70" s="15"/>
       <c r="N70" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="O70" s="18" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.4">
@@ -5502,6 +5462,12 @@
       <c r="F71" s="15"/>
       <c r="G71" s="12"/>
       <c r="J71" s="15"/>
+      <c r="N71" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="O71" s="18" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A72" s="14"/>
@@ -5515,6 +5481,12 @@
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
       <c r="J73" s="15"/>
+      <c r="N73" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="O73" s="29" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A74" s="15"/>
@@ -5523,6 +5495,12 @@
       <c r="F74" s="12"/>
       <c r="G74" s="15"/>
       <c r="J74" s="15"/>
+      <c r="N74" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="O74" s="27" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A75" s="15"/>
@@ -5531,10 +5509,22 @@
       <c r="H75" s="13"/>
       <c r="I75" s="15"/>
       <c r="L75" s="15"/>
+      <c r="N75" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="O75" s="27" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A76" s="15"/>
       <c r="B76" s="15"/>
+      <c r="N76" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="O76" s="27" t="s">
+        <v>285</v>
+      </c>
       <c r="U76" s="15"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.4">
@@ -5547,8 +5537,12 @@
       <c r="K77" s="14"/>
       <c r="L77" s="14"/>
       <c r="M77" s="14"/>
-      <c r="N77" s="14"/>
-      <c r="O77" s="14"/>
+      <c r="N77" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="O77" s="27" t="s">
+        <v>287</v>
+      </c>
       <c r="P77" s="14"/>
       <c r="Q77" s="14"/>
       <c r="R77" s="14"/>
@@ -5565,8 +5559,8 @@
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
       <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
       <c r="P78" s="15"/>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
@@ -5671,6 +5665,10 @@
       <c r="R84" s="15"/>
       <c r="S84" s="15"/>
       <c r="T84" s="15"/>
+    </row>
+    <row r="85" spans="7:20" x14ac:dyDescent="0.4">
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
@@ -5695,90 +5693,90 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D2" s="1">
         <v>23453</v>
@@ -5787,90 +5785,90 @@
         <v>45387</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>40</v>
@@ -5879,37 +5877,37 @@
         <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>40</v>
@@ -5918,7 +5916,7 @@
         <v>19</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>40</v>
@@ -5926,67 +5924,67 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D4" s="1">
         <v>30000</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>40</v>
@@ -5995,7 +5993,7 @@
         <v>19</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>40</v>
@@ -6003,28 +6001,28 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="D5" s="1">
         <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>40</v>
@@ -6033,37 +6031,37 @@
         <v>40</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>40</v>
@@ -6072,7 +6070,7 @@
         <v>19</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>40</v>
@@ -6080,67 +6078,67 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="D6" s="1">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>40</v>
@@ -6149,7 +6147,7 @@
         <v>19</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>40</v>
@@ -6157,25 +6155,25 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D7" s="1">
         <v>200</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>40</v>
@@ -6187,37 +6185,37 @@
         <v>40</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>40</v>
@@ -6226,7 +6224,7 @@
         <v>19</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>40</v>
@@ -6234,16 +6232,16 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>40</v>
@@ -6264,7 +6262,7 @@
         <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>40</v>
@@ -6273,7 +6271,7 @@
         <v>40</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>40</v>
@@ -6282,7 +6280,7 @@
         <v>40</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>40</v>
@@ -6291,7 +6289,7 @@
         <v>40</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>40</v>
@@ -6300,7 +6298,7 @@
         <v>40</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>40</v>
@@ -6311,10 +6309,10 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.4">
@@ -6322,7 +6320,7 @@
         <v>43</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="M12" s="1"/>
     </row>
@@ -6331,34 +6329,34 @@
         <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>231</v>
+        <v>207</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>224</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.4">
@@ -6366,24 +6364,24 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="D14" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="H14" s="32" t="s">
+      <c r="G14" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="H14" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L14" s="1">
@@ -6401,24 +6399,24 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="32" t="s">
+      <c r="D15" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="1">
@@ -6436,24 +6434,24 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D16" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="H16" s="32" t="s">
+      <c r="G16" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="H16" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L16" s="1">
@@ -6463,7 +6461,7 @@
         <v>2</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
@@ -6471,24 +6469,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="E17" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="32" t="s">
+      <c r="F17" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L17" s="1">
@@ -6506,25 +6504,25 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="E18" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>227</v>
+      <c r="H18" s="31" t="s">
+        <v>220</v>
       </c>
       <c r="L18" s="1">
         <v>4</v>
@@ -6541,24 +6539,24 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L19" s="1">
@@ -6576,24 +6574,24 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L20" s="1">
@@ -6614,27 +6612,27 @@
         <v>3</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L22" s="1">
         <v>2</v>
@@ -6643,7 +6641,7 @@
         <v>3</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.4">
@@ -6651,19 +6649,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L23" s="1">
         <v>3</v>
@@ -6672,7 +6670,7 @@
         <v>3</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.4">
@@ -6680,16 +6678,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>19</v>
@@ -6701,7 +6699,7 @@
         <v>3</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.4">
@@ -6709,19 +6707,19 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L25" s="1">
         <v>5</v>
@@ -6730,7 +6728,7 @@
         <v>3</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.4">
@@ -6741,7 +6739,7 @@
         <v>3</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.4">
@@ -6752,12 +6750,12 @@
         <v>3</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.4">
@@ -6765,61 +6763,61 @@
         <v>43</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="I30" s="33" t="s">
-        <v>277</v>
+      <c r="I30" s="32" t="s">
+        <v>270</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>279</v>
+        <v>207</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>272</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>215</v>
+      <c r="D32" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -6845,18 +6843,18 @@
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="G33" s="32">
+      <c r="D33" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="G33" s="31">
         <v>1</v>
       </c>
       <c r="I33" s="1">
@@ -6874,31 +6872,31 @@
       <c r="P33" s="1">
         <v>45387</v>
       </c>
-      <c r="V33" s="34" t="s">
+      <c r="V33" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="W33" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="Z33" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA33" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="AB33" s="34" t="s">
-        <v>278</v>
+      <c r="W33" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z33" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA33" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="AB33" s="33" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="32" t="s">
         <v>209</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="F34" s="1">
         <v>4</v>
@@ -6906,10 +6904,10 @@
       <c r="G34" s="1">
         <v>1</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="31">
         <v>5</v>
       </c>
-      <c r="J34" s="32">
+      <c r="J34" s="31">
         <v>2</v>
       </c>
       <c r="N34" s="1">
@@ -6919,33 +6917,33 @@
         <v>2</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="V34" s="34">
-        <v>1</v>
-      </c>
-      <c r="W34" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z34" s="34">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="34">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="34" t="s">
-        <v>215</v>
+        <v>206</v>
+      </c>
+      <c r="V34" s="33">
+        <v>1</v>
+      </c>
+      <c r="W34" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z34" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="33">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D35" s="33" t="s">
-        <v>216</v>
+        <v>204</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F35" s="1">
         <v>5</v>
@@ -6953,10 +6951,10 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="I35" s="32">
-        <v>1</v>
-      </c>
-      <c r="J35" s="32">
+      <c r="I35" s="31">
+        <v>1</v>
+      </c>
+      <c r="J35" s="31">
         <v>2</v>
       </c>
       <c r="N35" s="1">
@@ -6968,31 +6966,31 @@
       <c r="P35" s="1">
         <v>30000</v>
       </c>
-      <c r="V35" s="34">
-        <v>2</v>
-      </c>
-      <c r="W35" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z35" s="34">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB35" s="34" t="s">
-        <v>215</v>
+      <c r="V35" s="33">
+        <v>2</v>
+      </c>
+      <c r="W35" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z35" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>216</v>
+        <v>205</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F36" s="1">
         <v>6</v>
@@ -7009,36 +7007,36 @@
       <c r="P36" s="1">
         <v>70</v>
       </c>
-      <c r="V36" s="34">
-        <v>3</v>
-      </c>
-      <c r="W36" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z36" s="34">
-        <v>2</v>
-      </c>
-      <c r="AA36" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB36" s="34" t="s">
-        <v>216</v>
+      <c r="V36" s="33">
+        <v>3</v>
+      </c>
+      <c r="W36" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z36" s="33">
+        <v>2</v>
+      </c>
+      <c r="AA36" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB36" s="33" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B37" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="D37" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="F37" s="32">
-        <v>1</v>
-      </c>
-      <c r="G37" s="32">
+      <c r="F37" s="31">
+        <v>1</v>
+      </c>
+      <c r="G37" s="31">
         <v>4</v>
       </c>
       <c r="N37" s="1">
@@ -7050,31 +7048,31 @@
       <c r="P37" s="1">
         <v>30</v>
       </c>
-      <c r="V37" s="34">
+      <c r="V37" s="33">
         <v>4</v>
       </c>
-      <c r="W37" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z37" s="34">
-        <v>3</v>
-      </c>
-      <c r="AA37" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB37" s="34" t="s">
-        <v>215</v>
+      <c r="W37" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z37" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA37" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB37" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B38" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D38" s="33" t="s">
-        <v>216</v>
+        <v>206</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F38" s="1">
         <v>3</v>
@@ -7091,20 +7089,20 @@
       <c r="P38" s="1">
         <v>200</v>
       </c>
-      <c r="V38" s="34">
+      <c r="V38" s="33">
         <v>5</v>
       </c>
-      <c r="W38" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z38" s="34">
+      <c r="W38" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z38" s="33">
         <v>4</v>
       </c>
-      <c r="AA38" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB38" s="34" t="s">
-        <v>215</v>
+      <c r="AA38" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB38" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.4">
@@ -7121,29 +7119,29 @@
         <v>3</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="V39" s="34">
+        <v>206</v>
+      </c>
+      <c r="V39" s="33">
         <v>6</v>
       </c>
-      <c r="W39" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z39" s="34">
+      <c r="W39" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z39" s="33">
         <v>5</v>
       </c>
-      <c r="AA39" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB39" s="34" t="s">
-        <v>215</v>
+      <c r="AA39" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB39" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="F40" s="32">
+      <c r="F40" s="31">
         <v>5</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G40" s="31">
         <v>3</v>
       </c>
       <c r="N40" s="1">
@@ -7153,29 +7151,29 @@
         <v>3</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="V40" s="34">
+        <v>206</v>
+      </c>
+      <c r="V40" s="33">
         <v>7</v>
       </c>
-      <c r="W40" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z40" s="34">
+      <c r="W40" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z40" s="33">
         <v>6</v>
       </c>
-      <c r="AA40" s="34">
-        <v>2</v>
-      </c>
-      <c r="AB40" s="34" t="s">
-        <v>215</v>
+      <c r="AA40" s="33">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="F41" s="32">
-        <v>1</v>
-      </c>
-      <c r="G41" s="32">
+      <c r="F41" s="31">
+        <v>1</v>
+      </c>
+      <c r="G41" s="31">
         <v>5</v>
       </c>
       <c r="N41" s="1">
@@ -7185,16 +7183,16 @@
         <v>3</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z41" s="34">
-        <v>1</v>
-      </c>
-      <c r="AA41" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB41" s="34" t="s">
-        <v>215</v>
+        <v>206</v>
+      </c>
+      <c r="Z41" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB41" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.4">
@@ -7211,23 +7209,23 @@
         <v>3</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z42" s="34">
-        <v>3</v>
-      </c>
-      <c r="AA42" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB42" s="34" t="s">
-        <v>215</v>
+        <v>206</v>
+      </c>
+      <c r="Z42" s="33">
+        <v>3</v>
+      </c>
+      <c r="AA42" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB42" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="F43" s="32">
+      <c r="F43" s="31">
         <v>5</v>
       </c>
-      <c r="G43" s="32">
+      <c r="G43" s="31">
         <v>6</v>
       </c>
       <c r="N43" s="1">
@@ -7237,16 +7235,16 @@
         <v>3</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z43" s="34">
+        <v>206</v>
+      </c>
+      <c r="Z43" s="33">
         <v>4</v>
       </c>
-      <c r="AA43" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB43" s="34" t="s">
-        <v>215</v>
+      <c r="AA43" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB43" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="2:28" x14ac:dyDescent="0.4">
@@ -7257,56 +7255,56 @@
         <v>3</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z44" s="34">
+        <v>206</v>
+      </c>
+      <c r="Z44" s="33">
         <v>5</v>
       </c>
-      <c r="AA44" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB44" s="34" t="s">
-        <v>215</v>
+      <c r="AA44" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB44" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="Z45" s="34">
+      <c r="Z45" s="33">
         <v>6</v>
       </c>
-      <c r="AA45" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB45" s="34" t="s">
-        <v>215</v>
+      <c r="AA45" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB45" s="33" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="2:28" x14ac:dyDescent="0.4">
       <c r="N46" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z46" s="34">
+        <v>193</v>
+      </c>
+      <c r="Z46" s="33">
         <v>7</v>
       </c>
-      <c r="AA46" s="34">
-        <v>3</v>
-      </c>
-      <c r="AB46" s="34" t="s">
-        <v>216</v>
+      <c r="AA46" s="33">
+        <v>3</v>
+      </c>
+      <c r="AB46" s="33" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.4">
@@ -7314,19 +7312,19 @@
         <v>1</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="2:28" x14ac:dyDescent="0.4">
@@ -7334,16 +7332,16 @@
         <v>2</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>19</v>
@@ -7354,24 +7352,24 @@
         <v>3</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
@@ -7379,10 +7377,10 @@
         <v>43</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="J53" s="1"/>
     </row>
@@ -7391,31 +7389,31 @@
         <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D54" s="33" t="s">
-        <v>279</v>
+        <v>207</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>272</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.4">
@@ -7423,13 +7421,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>215</v>
+      <c r="D55" s="32" t="s">
+        <v>208</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -7447,7 +7445,7 @@
         <v>23453</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
@@ -7455,13 +7453,13 @@
         <v>2</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D56" s="33" t="s">
-        <v>216</v>
+      <c r="D56" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F56" s="1">
         <v>2</v>
@@ -7479,7 +7477,7 @@
         <v>45387</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.4">
@@ -7487,13 +7485,13 @@
         <v>3</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D57" s="32" t="s">
         <v>209</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="F57" s="1">
         <v>4</v>
@@ -7508,10 +7506,10 @@
         <v>2</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.4">
@@ -7519,13 +7517,13 @@
         <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>216</v>
+        <v>204</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F58" s="1">
         <v>5</v>
@@ -7543,7 +7541,7 @@
         <v>30000</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.4">
@@ -7551,13 +7549,13 @@
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D59" s="33" t="s">
-        <v>216</v>
+        <v>205</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F59" s="1">
         <v>6</v>
@@ -7575,10 +7573,10 @@
         <v>70</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.4">
@@ -7586,13 +7584,13 @@
         <v>6</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="32" t="s">
         <v>209</v>
-      </c>
-      <c r="D60" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="F60" s="1">
         <v>2</v>
@@ -7610,7 +7608,7 @@
         <v>30</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.4">
@@ -7618,13 +7616,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D61" s="33" t="s">
-        <v>216</v>
+        <v>206</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="F61" s="1">
         <v>3</v>
@@ -7642,16 +7640,16 @@
         <v>200</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O61" s="6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="S61" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.4">
@@ -7668,19 +7666,19 @@
         <v>3</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O62" s="6" t="s">
         <v>19</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="S62" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.4">
@@ -7697,16 +7695,16 @@
         <v>3</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.4">
@@ -7717,16 +7715,16 @@
         <v>3</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="6:18" x14ac:dyDescent="0.4">
@@ -7737,21 +7735,21 @@
         <v>3</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O65" s="6" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="66" spans="6:18" x14ac:dyDescent="0.4">
-      <c r="F66" s="33" t="s">
-        <v>277</v>
+      <c r="F66" s="32" t="s">
+        <v>270</v>
       </c>
       <c r="I66" s="1">
         <v>6</v>
@@ -7760,13 +7758,13 @@
         <v>3</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" spans="6:18" x14ac:dyDescent="0.4">
@@ -7774,7 +7772,7 @@
         <v>42</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="I67" s="1">
         <v>7</v>
@@ -7783,10 +7781,10 @@
         <v>3</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="6:18" x14ac:dyDescent="0.4">
@@ -7805,25 +7803,25 @@
         <v>5</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="6:18" x14ac:dyDescent="0.4">
@@ -7831,22 +7829,22 @@
         <v>1</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="R70" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71" spans="6:18" x14ac:dyDescent="0.4">
@@ -7854,16 +7852,16 @@
         <v>2</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>19</v>
@@ -7874,19 +7872,19 @@
         <v>3</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -7909,10 +7907,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>

</xml_diff>